<commit_message>
Updated data sheet & chromedriver version
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="157">
   <si>
     <t>Table 1</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>Xyz@123</t>
+  </si>
+  <si>
+    <t>User Search</t>
+  </si>
+  <si>
+    <t>Val. User Search</t>
+  </si>
+  <si>
+    <t>Val. User Search_01</t>
   </si>
   <si>
     <t>Single coworker message</t>
@@ -656,7 +665,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -689,6 +698,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -737,13 +752,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>625099</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>139382</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>626284</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>293052</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
@@ -753,7 +768,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17198599" y="20839747"/>
+          <a:off x="17198599" y="21298852"/>
           <a:ext cx="1245786" cy="306706"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1880,7 +1895,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AB122"/>
+  <dimension ref="A1:AB125"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2062,11 +2077,11 @@
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
     </row>
-    <row r="6" ht="23.9" customHeight="1">
-      <c r="A6" t="s" s="7">
+    <row r="6" ht="12.05" customHeight="1">
+      <c r="A6" t="s" s="11">
         <v>10</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="B6" t="s" s="12">
         <v>11</v>
       </c>
       <c r="C6" t="s" s="7">
@@ -2078,24 +2093,12 @@
       <c r="E6" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="F6" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="J6" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s" s="7">
-        <v>17</v>
-      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -2114,10 +2117,10 @@
       <c r="AA6" s="8"/>
       <c r="AB6" s="8"/>
     </row>
-    <row r="7" ht="36.9" customHeight="1">
+    <row r="7" ht="12.05" customHeight="1">
       <c r="A7" s="5"/>
-      <c r="B7" t="s" s="7">
-        <v>18</v>
+      <c r="B7" t="s" s="12">
+        <v>12</v>
       </c>
       <c r="C7" t="s" s="7">
         <v>7</v>
@@ -2128,24 +2131,12 @@
       <c r="E7" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F7" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="K7" t="s" s="7">
-        <v>24</v>
-      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
@@ -2194,18 +2185,40 @@
       <c r="AA8" s="8"/>
       <c r="AB8" s="8"/>
     </row>
-    <row r="9" ht="12.05" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+    <row r="9" ht="23.9" customHeight="1">
+      <c r="A9" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s" s="7">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s" s="7">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -2224,43 +2237,39 @@
       <c r="AA9" s="8"/>
       <c r="AB9" s="8"/>
     </row>
-    <row r="10" ht="23.9" customHeight="1">
-      <c r="A10" t="s" s="7">
+    <row r="10" ht="36.9" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s" s="7">
         <v>25</v>
       </c>
-      <c r="B10" t="s" s="7">
+      <c r="J10" t="s" s="7">
         <v>26</v>
       </c>
-      <c r="C10" t="s" s="7">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s" s="7">
-        <v>4</v>
-      </c>
-      <c r="E10" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="F10" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="H10" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="I10" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="J10" t="s" s="7">
+      <c r="K10" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="K10" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s" s="7">
-        <v>17</v>
-      </c>
+      <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -2278,41 +2287,19 @@
       <c r="AA10" s="8"/>
       <c r="AB10" s="8"/>
     </row>
-    <row r="11" ht="36.9" customHeight="1">
+    <row r="11" ht="12.05" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s" s="10">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="G11" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="J11" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="K11" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="L11" t="s" s="7">
-        <v>24</v>
-      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -2362,10 +2349,10 @@
     </row>
     <row r="13" ht="23.9" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s" s="7">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s" s="7">
         <v>3</v>
@@ -2377,24 +2364,26 @@
         <v>5</v>
       </c>
       <c r="F13" t="s" s="7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s" s="7">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H13" t="s" s="7">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I13" t="s" s="7">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s" s="7">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K13" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="L13" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="L13" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -2412,10 +2401,10 @@
       <c r="AA13" s="8"/>
       <c r="AB13" s="8"/>
     </row>
-    <row r="14" ht="23.9" customHeight="1">
+    <row r="14" ht="36.9" customHeight="1">
       <c r="A14" s="5"/>
       <c r="B14" t="s" s="7">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s" s="7">
         <v>7</v>
@@ -2426,25 +2415,27 @@
       <c r="E14" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F14" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="G14" t="s" s="12">
-        <v>20</v>
+      <c r="F14" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s" s="14">
+        <v>23</v>
       </c>
       <c r="H14" t="s" s="7">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I14" t="s" s="7">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J14" t="s" s="7">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K14" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="L14" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="L14" t="s" s="7">
+        <v>27</v>
+      </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
@@ -2494,10 +2485,10 @@
     </row>
     <row r="16" ht="23.9" customHeight="1">
       <c r="A16" t="s" s="7">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s" s="7">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s" s="7">
         <v>3</v>
@@ -2509,15 +2500,23 @@
         <v>5</v>
       </c>
       <c r="F16" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="G16" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="I16" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="J16" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s" s="7">
+        <v>37</v>
+      </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
@@ -2539,7 +2538,7 @@
     <row r="17" ht="23.9" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" t="s" s="7">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s" s="7">
         <v>7</v>
@@ -2550,16 +2549,24 @@
       <c r="E17" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F17" t="s" s="7">
+      <c r="F17" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="G17" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="I17" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="J17" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="K17" t="s" s="7">
+        <v>40</v>
+      </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -2610,10 +2617,10 @@
     </row>
     <row r="19" ht="23.9" customHeight="1">
       <c r="A19" t="s" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s" s="7">
         <v>3</v>
@@ -2625,9 +2632,11 @@
         <v>5</v>
       </c>
       <c r="F19" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="G19" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="G19" t="s" s="7">
+        <v>43</v>
+      </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -2653,7 +2662,7 @@
     <row r="20" ht="23.9" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" t="s" s="7">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s" s="7">
         <v>7</v>
@@ -2665,9 +2674,11 @@
         <v>9</v>
       </c>
       <c r="F20" t="s" s="7">
-        <v>24</v>
-      </c>
-      <c r="G20" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="G20" t="s" s="7">
+        <v>45</v>
+      </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -2737,20 +2748,12 @@
         <v>5</v>
       </c>
       <c r="F22" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="G22" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="H22" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="I22" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="J22" t="s" s="7">
-        <v>17</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
@@ -2770,7 +2773,7 @@
       <c r="AA22" s="8"/>
       <c r="AB22" s="8"/>
     </row>
-    <row r="23" ht="36.9" customHeight="1">
+    <row r="23" ht="23.9" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" t="s" s="7">
         <v>48</v>
@@ -2784,21 +2787,13 @@
       <c r="E23" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F23" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="G23" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="H23" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="I23" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="J23" t="s" s="7">
-        <v>24</v>
-      </c>
+      <c r="F23" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
@@ -2850,10 +2845,10 @@
     </row>
     <row r="25" ht="23.9" customHeight="1">
       <c r="A25" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s" s="7">
         <v>50</v>
-      </c>
-      <c r="B25" t="s" s="7">
-        <v>51</v>
       </c>
       <c r="C25" t="s" s="7">
         <v>3</v>
@@ -2865,14 +2860,20 @@
         <v>5</v>
       </c>
       <c r="F25" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="G25" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="G25" t="s" s="7">
+        <v>16</v>
+      </c>
       <c r="H25" t="s" s="7">
-        <v>52</v>
-      </c>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="I25" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="J25" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
@@ -2892,10 +2893,10 @@
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
     </row>
-    <row r="26" ht="23.9" customHeight="1">
+    <row r="26" ht="36.9" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" t="s" s="7">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s" s="7">
         <v>7</v>
@@ -2906,15 +2907,21 @@
       <c r="E26" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F26" t="s" s="7">
-        <v>24</v>
-      </c>
-      <c r="G26" s="7"/>
+      <c r="F26" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s" s="14">
+        <v>23</v>
+      </c>
       <c r="H26" t="s" s="7">
-        <v>54</v>
-      </c>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+        <v>52</v>
+      </c>
+      <c r="I26" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s" s="7">
+        <v>27</v>
+      </c>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
@@ -2964,12 +2971,12 @@
       <c r="AA27" s="8"/>
       <c r="AB27" s="8"/>
     </row>
-    <row r="28" ht="36.9" customHeight="1">
-      <c r="A28" t="s" s="13">
-        <v>55</v>
+    <row r="28" ht="23.9" customHeight="1">
+      <c r="A28" t="s" s="7">
+        <v>53</v>
       </c>
       <c r="B28" t="s" s="7">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s" s="7">
         <v>3</v>
@@ -2981,10 +2988,12 @@
         <v>5</v>
       </c>
       <c r="F28" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" t="s" s="7">
+        <v>55</v>
+      </c>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -3006,10 +3015,10 @@
       <c r="AA28" s="8"/>
       <c r="AB28" s="8"/>
     </row>
-    <row r="29" ht="36.9" customHeight="1">
+    <row r="29" ht="23.9" customHeight="1">
       <c r="A29" s="5"/>
       <c r="B29" t="s" s="7">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s" s="7">
         <v>7</v>
@@ -3021,10 +3030,12 @@
         <v>9</v>
       </c>
       <c r="F29" t="s" s="7">
-        <v>24</v>
-      </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" t="s" s="7">
+        <v>57</v>
+      </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -3076,8 +3087,8 @@
       <c r="AA30" s="8"/>
       <c r="AB30" s="8"/>
     </row>
-    <row r="31" ht="24.05" customHeight="1">
-      <c r="A31" t="s" s="13">
+    <row r="31" ht="36.9" customHeight="1">
+      <c r="A31" t="s" s="15">
         <v>58</v>
       </c>
       <c r="B31" t="s" s="7">
@@ -3093,7 +3104,7 @@
         <v>5</v>
       </c>
       <c r="F31" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -3118,7 +3129,7 @@
       <c r="AA31" s="8"/>
       <c r="AB31" s="8"/>
     </row>
-    <row r="32" ht="23.9" customHeight="1">
+    <row r="32" ht="36.9" customHeight="1">
       <c r="A32" s="5"/>
       <c r="B32" t="s" s="7">
         <v>60</v>
@@ -3133,7 +3144,7 @@
         <v>9</v>
       </c>
       <c r="F32" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
@@ -3188,8 +3199,8 @@
       <c r="AA33" s="8"/>
       <c r="AB33" s="8"/>
     </row>
-    <row r="34" ht="36.9" customHeight="1">
-      <c r="A34" t="s" s="13">
+    <row r="34" ht="24.05" customHeight="1">
+      <c r="A34" t="s" s="15">
         <v>61</v>
       </c>
       <c r="B34" t="s" s="7">
@@ -3205,7 +3216,7 @@
         <v>5</v>
       </c>
       <c r="F34" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
@@ -3230,7 +3241,7 @@
       <c r="AA34" s="8"/>
       <c r="AB34" s="8"/>
     </row>
-    <row r="35" ht="36.9" customHeight="1">
+    <row r="35" ht="23.9" customHeight="1">
       <c r="A35" s="5"/>
       <c r="B35" t="s" s="7">
         <v>63</v>
@@ -3245,7 +3256,7 @@
         <v>9</v>
       </c>
       <c r="F35" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
@@ -3301,7 +3312,7 @@
       <c r="AB36" s="8"/>
     </row>
     <row r="37" ht="36.9" customHeight="1">
-      <c r="A37" t="s" s="13">
+      <c r="A37" t="s" s="15">
         <v>64</v>
       </c>
       <c r="B37" t="s" s="7">
@@ -3317,7 +3328,7 @@
         <v>5</v>
       </c>
       <c r="F37" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
@@ -3357,7 +3368,7 @@
         <v>9</v>
       </c>
       <c r="F38" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -3412,8 +3423,8 @@
       <c r="AA39" s="8"/>
       <c r="AB39" s="8"/>
     </row>
-    <row r="40" ht="49.9" customHeight="1">
-      <c r="A40" t="s" s="13">
+    <row r="40" ht="36.9" customHeight="1">
+      <c r="A40" t="s" s="15">
         <v>67</v>
       </c>
       <c r="B40" t="s" s="7">
@@ -3429,7 +3440,7 @@
         <v>5</v>
       </c>
       <c r="F40" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
@@ -3454,7 +3465,7 @@
       <c r="AA40" s="8"/>
       <c r="AB40" s="8"/>
     </row>
-    <row r="41" ht="49.9" customHeight="1">
+    <row r="41" ht="36.9" customHeight="1">
       <c r="A41" s="5"/>
       <c r="B41" t="s" s="7">
         <v>69</v>
@@ -3469,7 +3480,7 @@
         <v>9</v>
       </c>
       <c r="F41" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
@@ -3524,8 +3535,8 @@
       <c r="AA42" s="8"/>
       <c r="AB42" s="8"/>
     </row>
-    <row r="43" ht="23.9" customHeight="1">
-      <c r="A43" t="s" s="7">
+    <row r="43" ht="49.9" customHeight="1">
+      <c r="A43" t="s" s="15">
         <v>70</v>
       </c>
       <c r="B43" t="s" s="7">
@@ -3541,23 +3552,13 @@
         <v>5</v>
       </c>
       <c r="F43" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="G43" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="H43" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="I43" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="J43" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="K43" t="s" s="7">
-        <v>17</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
@@ -3576,7 +3577,7 @@
       <c r="AA43" s="8"/>
       <c r="AB43" s="8"/>
     </row>
-    <row r="44" ht="23.9" customHeight="1">
+    <row r="44" ht="49.9" customHeight="1">
       <c r="A44" s="5"/>
       <c r="B44" t="s" s="7">
         <v>72</v>
@@ -3590,24 +3591,14 @@
       <c r="E44" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F44" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="G44" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="H44" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="I44" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="J44" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="K44" t="s" s="7">
-        <v>24</v>
-      </c>
+      <c r="F44" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
@@ -3656,7 +3647,7 @@
       <c r="AA45" s="8"/>
       <c r="AB45" s="8"/>
     </row>
-    <row r="46" ht="36.9" customHeight="1">
+    <row r="46" ht="23.9" customHeight="1">
       <c r="A46" t="s" s="7">
         <v>73</v>
       </c>
@@ -3673,22 +3664,22 @@
         <v>5</v>
       </c>
       <c r="F46" t="s" s="7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G46" t="s" s="7">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H46" t="s" s="7">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I46" t="s" s="7">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J46" t="s" s="7">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K46" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
@@ -3708,7 +3699,7 @@
       <c r="AA46" s="8"/>
       <c r="AB46" s="8"/>
     </row>
-    <row r="47" ht="36.9" customHeight="1">
+    <row r="47" ht="23.9" customHeight="1">
       <c r="A47" s="5"/>
       <c r="B47" t="s" s="7">
         <v>75</v>
@@ -3722,23 +3713,23 @@
       <c r="E47" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F47" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="G47" t="s" s="12">
-        <v>20</v>
+      <c r="F47" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="G47" t="s" s="14">
+        <v>23</v>
       </c>
       <c r="H47" t="s" s="7">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I47" t="s" s="7">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J47" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K47" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
@@ -3788,7 +3779,7 @@
       <c r="AA48" s="8"/>
       <c r="AB48" s="8"/>
     </row>
-    <row r="49" ht="23.9" customHeight="1">
+    <row r="49" ht="36.9" customHeight="1">
       <c r="A49" t="s" s="7">
         <v>76</v>
       </c>
@@ -3805,22 +3796,22 @@
         <v>5</v>
       </c>
       <c r="F49" t="s" s="7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G49" t="s" s="7">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H49" t="s" s="7">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I49" t="s" s="7">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J49" t="s" s="7">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K49" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
@@ -3840,7 +3831,7 @@
       <c r="AA49" s="8"/>
       <c r="AB49" s="8"/>
     </row>
-    <row r="50" ht="23.9" customHeight="1">
+    <row r="50" ht="36.9" customHeight="1">
       <c r="A50" s="5"/>
       <c r="B50" t="s" s="7">
         <v>78</v>
@@ -3854,23 +3845,23 @@
       <c r="E50" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F50" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="G50" t="s" s="12">
-        <v>20</v>
+      <c r="F50" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="G50" t="s" s="14">
+        <v>23</v>
       </c>
       <c r="H50" t="s" s="7">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I50" t="s" s="7">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J50" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K50" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
@@ -3937,22 +3928,22 @@
         <v>5</v>
       </c>
       <c r="F52" t="s" s="7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G52" t="s" s="7">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H52" t="s" s="7">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I52" t="s" s="7">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J52" t="s" s="7">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K52" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
@@ -3986,23 +3977,23 @@
       <c r="E53" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F53" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="G53" t="s" s="12">
-        <v>20</v>
+      <c r="F53" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="G53" t="s" s="14">
+        <v>23</v>
       </c>
       <c r="H53" t="s" s="7">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I53" t="s" s="7">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J53" t="s" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K53" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
@@ -4069,13 +4060,23 @@
         <v>5</v>
       </c>
       <c r="F55" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="G55" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="H55" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
+      <c r="I55" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="J55" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="K55" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
       <c r="N55" s="8"/>
@@ -4094,7 +4095,7 @@
       <c r="AA55" s="8"/>
       <c r="AB55" s="8"/>
     </row>
-    <row r="56" ht="36.9" customHeight="1">
+    <row r="56" ht="23.9" customHeight="1">
       <c r="A56" s="5"/>
       <c r="B56" t="s" s="7">
         <v>84</v>
@@ -4108,14 +4109,24 @@
       <c r="E56" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F56" t="s" s="7">
+      <c r="F56" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="G56" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="H56" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
+      <c r="I56" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J56" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="K56" t="s" s="7">
+        <v>27</v>
+      </c>
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
       <c r="N56" s="8"/>
@@ -4164,7 +4175,7 @@
       <c r="AA57" s="8"/>
       <c r="AB57" s="8"/>
     </row>
-    <row r="58" ht="36.9" customHeight="1">
+    <row r="58" ht="23.9" customHeight="1">
       <c r="A58" t="s" s="7">
         <v>85</v>
       </c>
@@ -4181,7 +4192,7 @@
         <v>5</v>
       </c>
       <c r="F58" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
@@ -4206,7 +4217,7 @@
       <c r="AA58" s="8"/>
       <c r="AB58" s="8"/>
     </row>
-    <row r="59" ht="23.9" customHeight="1">
+    <row r="59" ht="36.9" customHeight="1">
       <c r="A59" s="5"/>
       <c r="B59" t="s" s="7">
         <v>87</v>
@@ -4221,7 +4232,7 @@
         <v>9</v>
       </c>
       <c r="F59" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
@@ -4293,7 +4304,7 @@
         <v>5</v>
       </c>
       <c r="F61" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
@@ -4318,7 +4329,7 @@
       <c r="AA61" s="8"/>
       <c r="AB61" s="8"/>
     </row>
-    <row r="62" ht="36.9" customHeight="1">
+    <row r="62" ht="23.9" customHeight="1">
       <c r="A62" s="5"/>
       <c r="B62" t="s" s="7">
         <v>90</v>
@@ -4333,7 +4344,7 @@
         <v>9</v>
       </c>
       <c r="F62" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
@@ -4405,7 +4416,7 @@
         <v>5</v>
       </c>
       <c r="F64" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
@@ -4445,7 +4456,7 @@
         <v>9</v>
       </c>
       <c r="F65" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
@@ -4500,7 +4511,7 @@
       <c r="AA66" s="8"/>
       <c r="AB66" s="8"/>
     </row>
-    <row r="67" ht="23.9" customHeight="1">
+    <row r="67" ht="36.9" customHeight="1">
       <c r="A67" t="s" s="7">
         <v>94</v>
       </c>
@@ -4517,23 +4528,13 @@
         <v>5</v>
       </c>
       <c r="F67" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="G67" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="H67" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="I67" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="J67" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="K67" t="s" s="7">
-        <v>17</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8"/>
       <c r="L67" s="8"/>
       <c r="M67" s="8"/>
       <c r="N67" s="8"/>
@@ -4552,7 +4553,7 @@
       <c r="AA67" s="8"/>
       <c r="AB67" s="8"/>
     </row>
-    <row r="68" ht="23.9" customHeight="1">
+    <row r="68" ht="36.9" customHeight="1">
       <c r="A68" s="5"/>
       <c r="B68" t="s" s="7">
         <v>96</v>
@@ -4566,24 +4567,14 @@
       <c r="E68" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F68" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="G68" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="H68" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="I68" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="J68" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="K68" t="s" s="7">
-        <v>24</v>
-      </c>
+      <c r="F68" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
       <c r="L68" s="8"/>
       <c r="M68" s="8"/>
       <c r="N68" s="8"/>
@@ -4649,13 +4640,23 @@
         <v>5</v>
       </c>
       <c r="F70" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="G70" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="H70" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
+      <c r="I70" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="J70" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="K70" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="L70" s="8"/>
       <c r="M70" s="8"/>
       <c r="N70" s="8"/>
@@ -4688,14 +4689,24 @@
       <c r="E71" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F71" t="s" s="7">
+      <c r="F71" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="G71" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="H71" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8"/>
+      <c r="I71" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="J71" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="K71" t="s" s="7">
+        <v>27</v>
+      </c>
       <c r="L71" s="8"/>
       <c r="M71" s="8"/>
       <c r="N71" s="8"/>
@@ -4744,7 +4755,7 @@
       <c r="AA72" s="8"/>
       <c r="AB72" s="8"/>
     </row>
-    <row r="73" ht="49.9" customHeight="1">
+    <row r="73" ht="23.9" customHeight="1">
       <c r="A73" t="s" s="7">
         <v>100</v>
       </c>
@@ -4761,7 +4772,7 @@
         <v>5</v>
       </c>
       <c r="F73" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
@@ -4786,7 +4797,7 @@
       <c r="AA73" s="8"/>
       <c r="AB73" s="8"/>
     </row>
-    <row r="74" ht="49.9" customHeight="1">
+    <row r="74" ht="23.9" customHeight="1">
       <c r="A74" s="5"/>
       <c r="B74" t="s" s="7">
         <v>102</v>
@@ -4801,7 +4812,7 @@
         <v>9</v>
       </c>
       <c r="F74" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
@@ -4873,7 +4884,7 @@
         <v>5</v>
       </c>
       <c r="F76" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
@@ -4913,7 +4924,7 @@
         <v>9</v>
       </c>
       <c r="F77" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G77" s="8"/>
       <c r="H77" s="8"/>
@@ -4968,7 +4979,7 @@
       <c r="AA78" s="8"/>
       <c r="AB78" s="8"/>
     </row>
-    <row r="79" ht="36.9" customHeight="1">
+    <row r="79" ht="49.9" customHeight="1">
       <c r="A79" t="s" s="7">
         <v>106</v>
       </c>
@@ -4985,7 +4996,7 @@
         <v>5</v>
       </c>
       <c r="F79" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
@@ -5010,7 +5021,7 @@
       <c r="AA79" s="8"/>
       <c r="AB79" s="8"/>
     </row>
-    <row r="80" ht="36.9" customHeight="1">
+    <row r="80" ht="49.9" customHeight="1">
       <c r="A80" s="5"/>
       <c r="B80" t="s" s="7">
         <v>108</v>
@@ -5025,7 +5036,7 @@
         <v>9</v>
       </c>
       <c r="F80" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
@@ -5080,7 +5091,7 @@
       <c r="AA81" s="8"/>
       <c r="AB81" s="8"/>
     </row>
-    <row r="82" ht="23.9" customHeight="1">
+    <row r="82" ht="36.9" customHeight="1">
       <c r="A82" t="s" s="7">
         <v>109</v>
       </c>
@@ -5097,7 +5108,7 @@
         <v>5</v>
       </c>
       <c r="F82" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
@@ -5122,7 +5133,7 @@
       <c r="AA82" s="8"/>
       <c r="AB82" s="8"/>
     </row>
-    <row r="83" ht="23.9" customHeight="1">
+    <row r="83" ht="36.9" customHeight="1">
       <c r="A83" s="5"/>
       <c r="B83" t="s" s="7">
         <v>111</v>
@@ -5137,7 +5148,7 @@
         <v>9</v>
       </c>
       <c r="F83" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
@@ -5192,7 +5203,7 @@
       <c r="AA84" s="8"/>
       <c r="AB84" s="8"/>
     </row>
-    <row r="85" ht="36.9" customHeight="1">
+    <row r="85" ht="23.9" customHeight="1">
       <c r="A85" t="s" s="7">
         <v>112</v>
       </c>
@@ -5209,7 +5220,7 @@
         <v>5</v>
       </c>
       <c r="F85" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
@@ -5234,7 +5245,7 @@
       <c r="AA85" s="8"/>
       <c r="AB85" s="8"/>
     </row>
-    <row r="86" ht="36.9" customHeight="1">
+    <row r="86" ht="23.9" customHeight="1">
       <c r="A86" s="5"/>
       <c r="B86" t="s" s="7">
         <v>114</v>
@@ -5249,7 +5260,7 @@
         <v>9</v>
       </c>
       <c r="F86" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
@@ -5304,7 +5315,7 @@
       <c r="AA87" s="8"/>
       <c r="AB87" s="8"/>
     </row>
-    <row r="88" ht="12.05" customHeight="1">
+    <row r="88" ht="36.9" customHeight="1">
       <c r="A88" t="s" s="7">
         <v>115</v>
       </c>
@@ -5321,7 +5332,7 @@
         <v>5</v>
       </c>
       <c r="F88" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
@@ -5346,7 +5357,7 @@
       <c r="AA88" s="8"/>
       <c r="AB88" s="8"/>
     </row>
-    <row r="89" ht="23.9" customHeight="1">
+    <row r="89" ht="36.9" customHeight="1">
       <c r="A89" s="5"/>
       <c r="B89" t="s" s="7">
         <v>117</v>
@@ -5361,7 +5372,7 @@
         <v>9</v>
       </c>
       <c r="F89" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G89" s="8"/>
       <c r="H89" s="8"/>
@@ -5416,7 +5427,7 @@
       <c r="AA90" s="8"/>
       <c r="AB90" s="8"/>
     </row>
-    <row r="91" ht="49.9" customHeight="1">
+    <row r="91" ht="12.05" customHeight="1">
       <c r="A91" t="s" s="7">
         <v>118</v>
       </c>
@@ -5433,7 +5444,7 @@
         <v>5</v>
       </c>
       <c r="F91" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
@@ -5458,7 +5469,7 @@
       <c r="AA91" s="8"/>
       <c r="AB91" s="8"/>
     </row>
-    <row r="92" ht="49.9" customHeight="1">
+    <row r="92" ht="23.9" customHeight="1">
       <c r="A92" s="5"/>
       <c r="B92" t="s" s="7">
         <v>120</v>
@@ -5473,7 +5484,7 @@
         <v>9</v>
       </c>
       <c r="F92" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G92" s="8"/>
       <c r="H92" s="8"/>
@@ -5528,7 +5539,7 @@
       <c r="AA93" s="8"/>
       <c r="AB93" s="8"/>
     </row>
-    <row r="94" ht="36.9" customHeight="1">
+    <row r="94" ht="49.9" customHeight="1">
       <c r="A94" t="s" s="7">
         <v>121</v>
       </c>
@@ -5545,14 +5556,10 @@
         <v>5</v>
       </c>
       <c r="F94" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="G94" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="H94" t="s" s="7">
-        <v>14</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
       <c r="I94" s="8"/>
       <c r="J94" s="8"/>
       <c r="K94" s="8"/>
@@ -5574,7 +5581,7 @@
       <c r="AA94" s="8"/>
       <c r="AB94" s="8"/>
     </row>
-    <row r="95" ht="36.9" customHeight="1">
+    <row r="95" ht="49.9" customHeight="1">
       <c r="A95" s="5"/>
       <c r="B95" t="s" s="7">
         <v>123</v>
@@ -5589,14 +5596,10 @@
         <v>9</v>
       </c>
       <c r="F95" t="s" s="7">
-        <v>24</v>
-      </c>
-      <c r="G95" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="H95" t="s" s="7">
-        <v>21</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
       <c r="I95" s="8"/>
       <c r="J95" s="8"/>
       <c r="K95" s="8"/>
@@ -5665,17 +5668,15 @@
         <v>5</v>
       </c>
       <c r="F97" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="G97" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="H97" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="G97" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="H97" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="I97" t="s" s="7">
-        <v>15</v>
-      </c>
+      <c r="I97" s="8"/>
       <c r="J97" s="8"/>
       <c r="K97" s="8"/>
       <c r="L97" s="8"/>
@@ -5696,7 +5697,7 @@
       <c r="AA97" s="8"/>
       <c r="AB97" s="8"/>
     </row>
-    <row r="98" ht="23.9" customHeight="1">
+    <row r="98" ht="36.9" customHeight="1">
       <c r="A98" s="5"/>
       <c r="B98" t="s" s="7">
         <v>126</v>
@@ -5711,17 +5712,15 @@
         <v>9</v>
       </c>
       <c r="F98" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="G98" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="H98" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="G98" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="H98" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="I98" t="s" s="7">
-        <v>127</v>
-      </c>
+      <c r="I98" s="8"/>
       <c r="J98" s="8"/>
       <c r="K98" s="8"/>
       <c r="L98" s="8"/>
@@ -5774,10 +5773,10 @@
     </row>
     <row r="100" ht="36.9" customHeight="1">
       <c r="A100" t="s" s="7">
+        <v>127</v>
+      </c>
+      <c r="B100" t="s" s="7">
         <v>128</v>
-      </c>
-      <c r="B100" t="s" s="7">
-        <v>129</v>
       </c>
       <c r="C100" t="s" s="7">
         <v>3</v>
@@ -5789,15 +5788,17 @@
         <v>5</v>
       </c>
       <c r="F100" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="G100" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="H100" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="G100" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="H100" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="I100" s="8"/>
+      <c r="I100" t="s" s="7">
+        <v>18</v>
+      </c>
       <c r="J100" s="8"/>
       <c r="K100" s="8"/>
       <c r="L100" s="8"/>
@@ -5818,10 +5819,10 @@
       <c r="AA100" s="8"/>
       <c r="AB100" s="8"/>
     </row>
-    <row r="101" ht="36.9" customHeight="1">
+    <row r="101" ht="23.9" customHeight="1">
       <c r="A101" s="5"/>
       <c r="B101" t="s" s="7">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C101" t="s" s="7">
         <v>7</v>
@@ -5833,15 +5834,17 @@
         <v>9</v>
       </c>
       <c r="F101" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="G101" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="H101" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="G101" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="H101" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="I101" s="8"/>
+      <c r="I101" t="s" s="7">
+        <v>130</v>
+      </c>
       <c r="J101" s="8"/>
       <c r="K101" s="8"/>
       <c r="L101" s="8"/>
@@ -5909,17 +5912,15 @@
         <v>5</v>
       </c>
       <c r="F103" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="G103" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="H103" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="G103" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="H103" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="I103" t="s" s="7">
-        <v>15</v>
-      </c>
+      <c r="I103" s="8"/>
       <c r="J103" s="8"/>
       <c r="K103" s="8"/>
       <c r="L103" s="8"/>
@@ -5940,7 +5941,7 @@
       <c r="AA103" s="8"/>
       <c r="AB103" s="8"/>
     </row>
-    <row r="104" ht="23.9" customHeight="1">
+    <row r="104" ht="36.9" customHeight="1">
       <c r="A104" s="5"/>
       <c r="B104" t="s" s="7">
         <v>133</v>
@@ -5955,18 +5956,16 @@
         <v>9</v>
       </c>
       <c r="F104" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="G104" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="H104" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="G104" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="H104" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="I104" t="s" s="14">
-        <v>22</v>
-      </c>
-      <c r="J104" s="15"/>
+      <c r="I104" s="8"/>
+      <c r="J104" s="8"/>
       <c r="K104" s="8"/>
       <c r="L104" s="8"/>
       <c r="M104" s="8"/>
@@ -6033,15 +6032,17 @@
         <v>5</v>
       </c>
       <c r="F106" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="G106" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="H106" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="G106" t="s" s="7">
-        <v>136</v>
-      </c>
-      <c r="H106" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="I106" s="8"/>
+      <c r="I106" t="s" s="7">
+        <v>18</v>
+      </c>
       <c r="J106" s="8"/>
       <c r="K106" s="8"/>
       <c r="L106" s="8"/>
@@ -6062,10 +6063,10 @@
       <c r="AA106" s="8"/>
       <c r="AB106" s="8"/>
     </row>
-    <row r="107" ht="49.9" customHeight="1">
+    <row r="107" ht="23.9" customHeight="1">
       <c r="A107" s="5"/>
       <c r="B107" t="s" s="7">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C107" t="s" s="7">
         <v>7</v>
@@ -6077,16 +6078,18 @@
         <v>9</v>
       </c>
       <c r="F107" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="G107" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="H107" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="G107" t="s" s="7">
-        <v>138</v>
-      </c>
-      <c r="H107" t="s" s="7">
-        <v>21</v>
-      </c>
-      <c r="I107" s="8"/>
-      <c r="J107" s="8"/>
+      <c r="I107" t="s" s="16">
+        <v>25</v>
+      </c>
+      <c r="J107" s="17"/>
       <c r="K107" s="8"/>
       <c r="L107" s="8"/>
       <c r="M107" s="8"/>
@@ -6136,12 +6139,12 @@
       <c r="AA108" s="8"/>
       <c r="AB108" s="8"/>
     </row>
-    <row r="109" ht="49.9" customHeight="1">
+    <row r="109" ht="36.9" customHeight="1">
       <c r="A109" t="s" s="7">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B109" t="s" s="7">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C109" t="s" s="7">
         <v>3</v>
@@ -6153,12 +6156,14 @@
         <v>5</v>
       </c>
       <c r="F109" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="G109" t="s" s="7">
+        <v>139</v>
+      </c>
+      <c r="H109" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="G109" t="s" s="7">
-        <v>136</v>
-      </c>
-      <c r="H109" s="8"/>
       <c r="I109" s="8"/>
       <c r="J109" s="8"/>
       <c r="K109" s="8"/>
@@ -6183,7 +6188,7 @@
     <row r="110" ht="49.9" customHeight="1">
       <c r="A110" s="5"/>
       <c r="B110" t="s" s="7">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C110" t="s" s="7">
         <v>7</v>
@@ -6195,12 +6200,14 @@
         <v>9</v>
       </c>
       <c r="F110" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="G110" t="s" s="7">
+        <v>141</v>
+      </c>
+      <c r="H110" t="s" s="7">
         <v>24</v>
       </c>
-      <c r="G110" t="s" s="7">
-        <v>138</v>
-      </c>
-      <c r="H110" s="8"/>
       <c r="I110" s="8"/>
       <c r="J110" s="8"/>
       <c r="K110" s="8"/>
@@ -6269,10 +6276,10 @@
         <v>5</v>
       </c>
       <c r="F112" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G112" t="s" s="7">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H112" s="8"/>
       <c r="I112" s="8"/>
@@ -6296,7 +6303,7 @@
       <c r="AA112" s="8"/>
       <c r="AB112" s="8"/>
     </row>
-    <row r="113" ht="62.9" customHeight="1">
+    <row r="113" ht="49.9" customHeight="1">
       <c r="A113" s="5"/>
       <c r="B113" t="s" s="7">
         <v>144</v>
@@ -6311,10 +6318,10 @@
         <v>9</v>
       </c>
       <c r="F113" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G113" t="s" s="7">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H113" s="8"/>
       <c r="I113" s="8"/>
@@ -6385,10 +6392,10 @@
         <v>5</v>
       </c>
       <c r="F115" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G115" t="s" s="7">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H115" s="8"/>
       <c r="I115" s="8"/>
@@ -6412,7 +6419,7 @@
       <c r="AA115" s="8"/>
       <c r="AB115" s="8"/>
     </row>
-    <row r="116" ht="49.9" customHeight="1">
+    <row r="116" ht="62.9" customHeight="1">
       <c r="A116" s="5"/>
       <c r="B116" t="s" s="7">
         <v>147</v>
@@ -6427,10 +6434,10 @@
         <v>9</v>
       </c>
       <c r="F116" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G116" t="s" s="7">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H116" s="8"/>
       <c r="I116" s="8"/>
@@ -6484,7 +6491,7 @@
       <c r="AA117" s="8"/>
       <c r="AB117" s="8"/>
     </row>
-    <row r="118" ht="75.9" customHeight="1">
+    <row r="118" ht="49.9" customHeight="1">
       <c r="A118" t="s" s="7">
         <v>148</v>
       </c>
@@ -6501,14 +6508,12 @@
         <v>5</v>
       </c>
       <c r="F118" t="s" s="7">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G118" t="s" s="7">
-        <v>136</v>
-      </c>
-      <c r="H118" t="s" s="7">
-        <v>16</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="H118" s="8"/>
       <c r="I118" s="8"/>
       <c r="J118" s="8"/>
       <c r="K118" s="8"/>
@@ -6530,7 +6535,7 @@
       <c r="AA118" s="8"/>
       <c r="AB118" s="8"/>
     </row>
-    <row r="119" ht="75.9" customHeight="1">
+    <row r="119" ht="49.9" customHeight="1">
       <c r="A119" s="5"/>
       <c r="B119" t="s" s="7">
         <v>150</v>
@@ -6545,14 +6550,12 @@
         <v>9</v>
       </c>
       <c r="F119" t="s" s="7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G119" t="s" s="7">
-        <v>138</v>
-      </c>
-      <c r="H119" t="s" s="7">
-        <v>23</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H119" s="8"/>
       <c r="I119" s="8"/>
       <c r="J119" s="8"/>
       <c r="K119" s="8"/>
@@ -6604,7 +6607,7 @@
       <c r="AA120" s="8"/>
       <c r="AB120" s="8"/>
     </row>
-    <row r="121" ht="36.9" customHeight="1">
+    <row r="121" ht="75.9" customHeight="1">
       <c r="A121" t="s" s="7">
         <v>151</v>
       </c>
@@ -6621,10 +6624,14 @@
         <v>5</v>
       </c>
       <c r="F121" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="G121" s="8"/>
-      <c r="H121" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="G121" t="s" s="7">
+        <v>139</v>
+      </c>
+      <c r="H121" t="s" s="7">
+        <v>19</v>
+      </c>
       <c r="I121" s="8"/>
       <c r="J121" s="8"/>
       <c r="K121" s="8"/>
@@ -6646,7 +6653,7 @@
       <c r="AA121" s="8"/>
       <c r="AB121" s="8"/>
     </row>
-    <row r="122" ht="23.9" customHeight="1">
+    <row r="122" ht="75.9" customHeight="1">
       <c r="A122" s="5"/>
       <c r="B122" t="s" s="7">
         <v>153</v>
@@ -6661,10 +6668,14 @@
         <v>9</v>
       </c>
       <c r="F122" t="s" s="7">
-        <v>24</v>
-      </c>
-      <c r="G122" s="8"/>
-      <c r="H122" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="G122" t="s" s="7">
+        <v>141</v>
+      </c>
+      <c r="H122" t="s" s="7">
+        <v>26</v>
+      </c>
       <c r="I122" s="8"/>
       <c r="J122" s="8"/>
       <c r="K122" s="8"/>
@@ -6686,44 +6697,156 @@
       <c r="AA122" s="8"/>
       <c r="AB122" s="8"/>
     </row>
+    <row r="123" ht="12.05" customHeight="1">
+      <c r="A123" s="5"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
+      <c r="F123" s="8"/>
+      <c r="G123" s="8"/>
+      <c r="H123" s="8"/>
+      <c r="I123" s="8"/>
+      <c r="J123" s="8"/>
+      <c r="K123" s="8"/>
+      <c r="L123" s="8"/>
+      <c r="M123" s="8"/>
+      <c r="N123" s="8"/>
+      <c r="O123" s="8"/>
+      <c r="P123" s="8"/>
+      <c r="Q123" s="8"/>
+      <c r="R123" s="8"/>
+      <c r="S123" s="8"/>
+      <c r="T123" s="8"/>
+      <c r="U123" s="8"/>
+      <c r="V123" s="8"/>
+      <c r="W123" s="8"/>
+      <c r="X123" s="8"/>
+      <c r="Y123" s="8"/>
+      <c r="Z123" s="8"/>
+      <c r="AA123" s="8"/>
+      <c r="AB123" s="8"/>
+    </row>
+    <row r="124" ht="36.9" customHeight="1">
+      <c r="A124" t="s" s="7">
+        <v>154</v>
+      </c>
+      <c r="B124" t="s" s="7">
+        <v>155</v>
+      </c>
+      <c r="C124" t="s" s="7">
+        <v>3</v>
+      </c>
+      <c r="D124" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="E124" t="s" s="7">
+        <v>5</v>
+      </c>
+      <c r="F124" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="G124" s="8"/>
+      <c r="H124" s="8"/>
+      <c r="I124" s="8"/>
+      <c r="J124" s="8"/>
+      <c r="K124" s="8"/>
+      <c r="L124" s="8"/>
+      <c r="M124" s="8"/>
+      <c r="N124" s="8"/>
+      <c r="O124" s="8"/>
+      <c r="P124" s="8"/>
+      <c r="Q124" s="8"/>
+      <c r="R124" s="8"/>
+      <c r="S124" s="8"/>
+      <c r="T124" s="8"/>
+      <c r="U124" s="8"/>
+      <c r="V124" s="8"/>
+      <c r="W124" s="8"/>
+      <c r="X124" s="8"/>
+      <c r="Y124" s="8"/>
+      <c r="Z124" s="8"/>
+      <c r="AA124" s="8"/>
+      <c r="AB124" s="8"/>
+    </row>
+    <row r="125" ht="23.9" customHeight="1">
+      <c r="A125" s="5"/>
+      <c r="B125" t="s" s="7">
+        <v>156</v>
+      </c>
+      <c r="C125" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="D125" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="E125" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="F125" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="G125" s="8"/>
+      <c r="H125" s="8"/>
+      <c r="I125" s="8"/>
+      <c r="J125" s="8"/>
+      <c r="K125" s="8"/>
+      <c r="L125" s="8"/>
+      <c r="M125" s="8"/>
+      <c r="N125" s="8"/>
+      <c r="O125" s="8"/>
+      <c r="P125" s="8"/>
+      <c r="Q125" s="8"/>
+      <c r="R125" s="8"/>
+      <c r="S125" s="8"/>
+      <c r="T125" s="8"/>
+      <c r="U125" s="8"/>
+      <c r="V125" s="8"/>
+      <c r="W125" s="8"/>
+      <c r="X125" s="8"/>
+      <c r="Y125" s="8"/>
+      <c r="Z125" s="8"/>
+      <c r="AA125" s="8"/>
+      <c r="AB125" s="8"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:AB1"/>
-    <mergeCell ref="I104:J104"/>
+    <mergeCell ref="I107:J107"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D7" r:id="rId2" location="" tooltip="" display="shijinsureshv@gmail.com"/>
-    <hyperlink ref="F7" r:id="rId3" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
-    <hyperlink ref="D11" r:id="rId4" location="" tooltip="" display="shijinsureshv@gmail.com"/>
-    <hyperlink ref="F11" r:id="rId5" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
-    <hyperlink ref="D14" r:id="rId6" location="" tooltip="" display="shijinsureshv@gmail.com"/>
-    <hyperlink ref="F14" r:id="rId7" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
-    <hyperlink ref="D17" r:id="rId8" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="D10" r:id="rId3" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="F10" r:id="rId4" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
+    <hyperlink ref="D14" r:id="rId5" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="F14" r:id="rId6" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
+    <hyperlink ref="D17" r:id="rId7" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="F17" r:id="rId8" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
     <hyperlink ref="D20" r:id="rId9" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D23" r:id="rId10" location="" tooltip="" display="shijinsureshv@gmail.com"/>
-    <hyperlink ref="F23" r:id="rId11" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
-    <hyperlink ref="D26" r:id="rId12" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="D26" r:id="rId11" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="F26" r:id="rId12" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
     <hyperlink ref="D29" r:id="rId13" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D32" r:id="rId14" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D35" r:id="rId15" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D38" r:id="rId16" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D41" r:id="rId17" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D44" r:id="rId18" location="" tooltip="" display="shijinsureshv@gmail.com"/>
-    <hyperlink ref="F44" r:id="rId19" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
-    <hyperlink ref="D47" r:id="rId20" location="" tooltip="" display="shijinsureshv@gmail.com"/>
-    <hyperlink ref="F47" r:id="rId21" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
-    <hyperlink ref="D50" r:id="rId22" location="" tooltip="" display="shijinsureshv@gmail.com"/>
-    <hyperlink ref="F50" r:id="rId23" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
-    <hyperlink ref="D53" r:id="rId24" location="" tooltip="" display="shijinsureshv@gmail.com"/>
-    <hyperlink ref="F53" r:id="rId25" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
-    <hyperlink ref="D56" r:id="rId26" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="D47" r:id="rId19" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="F47" r:id="rId20" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
+    <hyperlink ref="D50" r:id="rId21" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="F50" r:id="rId22" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
+    <hyperlink ref="D53" r:id="rId23" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="F53" r:id="rId24" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
+    <hyperlink ref="D56" r:id="rId25" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="F56" r:id="rId26" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
     <hyperlink ref="D59" r:id="rId27" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D62" r:id="rId28" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D65" r:id="rId29" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D68" r:id="rId30" location="" tooltip="" display="shijinsureshv@gmail.com"/>
-    <hyperlink ref="F68" r:id="rId31" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
-    <hyperlink ref="D71" r:id="rId32" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="D71" r:id="rId31" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="F71" r:id="rId32" location="" tooltip="" display="surabhis+0989@geekyants.com"/>
     <hyperlink ref="D74" r:id="rId33" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D77" r:id="rId34" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D80" r:id="rId35" location="" tooltip="" display="shijinsureshv@gmail.com"/>
@@ -6741,12 +6864,13 @@
     <hyperlink ref="D116" r:id="rId47" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D119" r:id="rId48" location="" tooltip="" display="shijinsureshv@gmail.com"/>
     <hyperlink ref="D122" r:id="rId49" location="" tooltip="" display="shijinsureshv@gmail.com"/>
+    <hyperlink ref="D125" r:id="rId50" location="" tooltip="" display="shijinsureshv@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId50"/>
+  <drawing r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>